<commit_message>
More test and minor bugfixes
</commit_message>
<xml_diff>
--- a/Docs/AHPL/CSR.xlsx
+++ b/Docs/AHPL/CSR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\RISC-V-Processor-AHPL\Docs\AHPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACA8E62-A6BC-4983-9E56-2645D8E7ADF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D877911B-932B-438D-BD97-7B6589C5B7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{86CAE48D-CDE6-43A5-BCA4-CFB2646DD800}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="100">
   <si>
     <t>0x</t>
   </si>
@@ -497,12 +497,15 @@
   <si>
     <t>R MW</t>
   </si>
+  <si>
+    <t>Csr Test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -548,8 +551,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,6 +596,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -949,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1096,6 +1112,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,9 +1151,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1516,23 +1539,23 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="67" t="s">
+      <c r="C2" s="65"/>
+      <c r="D2" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="57" t="s">
         <v>47</v>
       </c>
       <c r="I2" s="5"/>
@@ -1542,13 +1565,13 @@
       <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="65"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="57"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="58"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1930,7 +1953,7 @@
       <c r="G14" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="58" t="s">
+      <c r="H14" s="59" t="s">
         <v>75</v>
       </c>
       <c r="I14" s="5">
@@ -1965,7 +1988,7 @@
       <c r="G15" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="59"/>
+      <c r="H15" s="60"/>
       <c r="I15" s="5">
         <f t="shared" si="1"/>
         <v>776</v>
@@ -1998,7 +2021,7 @@
       <c r="G16" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="59"/>
+      <c r="H16" s="60"/>
       <c r="I16" s="5">
         <f t="shared" si="1"/>
         <v>777</v>
@@ -2031,7 +2054,7 @@
       <c r="G17" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="60"/>
+      <c r="H17" s="61"/>
       <c r="I17" s="5">
         <f t="shared" si="1"/>
         <v>778</v>
@@ -2318,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9C5A5-BA11-4A2E-A79A-6B42F00E1AC0}">
-  <dimension ref="B2:X22"/>
+  <dimension ref="B2:AB22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:V13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2335,7 +2358,7 @@
     <col min="25" max="26" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E2" s="37">
         <v>18</v>
       </c>
@@ -2394,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="43" t="s">
         <v>79</v>
       </c>
@@ -2465,7 +2488,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B4" s="38">
         <v>3857</v>
       </c>
@@ -2536,7 +2559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B5" s="39">
         <v>3858</v>
       </c>
@@ -2607,7 +2630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B6" s="39">
         <v>3859</v>
       </c>
@@ -2678,7 +2701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B7" s="39">
         <v>3860</v>
       </c>
@@ -2749,7 +2772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B8" s="39">
         <v>769</v>
       </c>
@@ -2819,8 +2842,11 @@
       <c r="X8" s="17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AA8" s="69" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B9" s="39">
         <v>768</v>
       </c>
@@ -2890,8 +2916,9 @@
       <c r="X9" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AA9" s="69"/>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B10" s="40">
         <v>833</v>
       </c>
@@ -2961,8 +2988,9 @@
       <c r="X10" s="21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AA10" s="69"/>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B11" s="40">
         <v>835</v>
       </c>
@@ -3032,8 +3060,9 @@
       <c r="X11" s="21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AA11" s="69"/>
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B12" s="41">
         <v>772</v>
       </c>
@@ -3103,8 +3132,9 @@
       <c r="X12" s="25" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AA12" s="69"/>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B13" s="41">
         <v>836</v>
       </c>
@@ -3144,28 +3174,28 @@
       <c r="N13" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="O13" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="P13" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q13" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="R13" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="S13" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="T13" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="U13" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="V13" s="68" t="s">
+      <c r="O13" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="P13" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q13" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="R13" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="S13" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="T13" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="U13" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="V13" s="56" t="s">
         <v>83</v>
       </c>
       <c r="W13" s="49" t="s">
@@ -3175,7 +3205,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B14" s="41">
         <v>775</v>
       </c>
@@ -3245,8 +3275,11 @@
       <c r="X14" s="25" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AA14" s="70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B15" s="41">
         <v>776</v>
       </c>
@@ -3316,8 +3349,9 @@
       <c r="X15" s="25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="AB15" s="71"/>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B16" s="41">
         <v>777</v>
       </c>
@@ -3629,6 +3663,9 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C7:D28">
     <sortCondition descending="1" ref="C7"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="AA8:AA12"/>
+  </mergeCells>
   <conditionalFormatting sqref="P21:W21 I22:X22 W18:W19 T19:T20 U20:W20 H18:H22 O18:O21 E4:W17 P18:V18 I18:N18">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"N"</formula>

</xml_diff>